<commit_message>
Eliminación de Recursos 11_16
Eliminación de Recursos 11_16
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion16/Escaleta_CN_11_16_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion16/Escaleta_CN_11_16_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado11\guion16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado11\guion16\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -697,7 +697,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +776,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -833,7 +839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -907,16 +913,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -958,23 +982,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1298,126 +1321,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U286"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I3:I24"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.86328125" customWidth="1"/>
-    <col min="3" max="3" width="50.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.86328125" customWidth="1"/>
-    <col min="5" max="5" width="32.86328125" customWidth="1"/>
-    <col min="6" max="6" width="11.59765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="57.73046875" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="114.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.265625" customWidth="1"/>
-    <col min="12" max="12" width="17.3984375" customWidth="1"/>
-    <col min="13" max="14" width="9.265625" customWidth="1"/>
-    <col min="15" max="15" width="37.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.53125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.9296875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.1328125" customWidth="1"/>
-    <col min="19" max="19" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.86328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="57.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="114.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="27" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:21" s="27" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="37" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="37" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="27" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44"/>
+    <row r="2" spans="1:21" s="27" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="28" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="38"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
@@ -1474,7 +1497,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -1507,7 +1530,7 @@
       <c r="T4" s="12"/>
       <c r="U4" s="10"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>17</v>
       </c>
@@ -1568,7 +1591,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
@@ -1629,7 +1652,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>17</v>
       </c>
@@ -1662,7 +1685,7 @@
       <c r="T7" s="12"/>
       <c r="U7" s="10"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
@@ -1723,66 +1746,66 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16" t="s">
+      <c r="F9" s="60"/>
+      <c r="G9" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="61">
         <v>5</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8" t="s">
+      <c r="M9" s="62"/>
+      <c r="N9" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9" t="s">
+      <c r="O9" s="60"/>
+      <c r="P9" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="60">
         <v>6</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="R9" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="S9" s="10" t="s">
+      <c r="S9" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="U9" s="60" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
@@ -1841,7 +1864,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
@@ -1898,7 +1921,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>17</v>
       </c>
@@ -1931,7 +1954,7 @@
       <c r="T12" s="12"/>
       <c r="U12" s="10"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>17</v>
       </c>
@@ -1990,7 +2013,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>17</v>
       </c>
@@ -2049,7 +2072,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -2108,7 +2131,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -2141,7 +2164,7 @@
       <c r="T16" s="12"/>
       <c r="U16" s="10"/>
     </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>17</v>
       </c>
@@ -2174,7 +2197,7 @@
       <c r="T17" s="12"/>
       <c r="U17" s="10"/>
     </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>17</v>
       </c>
@@ -2233,7 +2256,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>17</v>
       </c>
@@ -2292,7 +2315,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
@@ -2349,64 +2372,64 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="16" t="s">
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="61">
         <v>14</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="J21" s="64" t="s">
         <v>190</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K21" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8" t="s">
+      <c r="M21" s="62"/>
+      <c r="N21" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9" t="s">
+      <c r="O21" s="60"/>
+      <c r="P21" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="Q21" s="60">
         <v>6</v>
       </c>
-      <c r="R21" s="11" t="s">
+      <c r="R21" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="S21" s="10" t="s">
+      <c r="S21" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="T21" s="12" t="s">
+      <c r="T21" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="U21" s="10" t="s">
+      <c r="U21" s="60" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>17</v>
       </c>
@@ -2451,7 +2474,7 @@
       <c r="T22" s="12"/>
       <c r="U22" s="10"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>17</v>
       </c>
@@ -2508,7 +2531,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>17</v>
       </c>
@@ -2563,7 +2586,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14"/>
@@ -2586,7 +2609,7 @@
       <c r="T25" s="12"/>
       <c r="U25" s="10"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14"/>
@@ -2609,7 +2632,7 @@
       <c r="T26" s="12"/>
       <c r="U26" s="10"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
@@ -2632,7 +2655,7 @@
       <c r="T27" s="12"/>
       <c r="U27" s="10"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14"/>
@@ -2655,7 +2678,7 @@
       <c r="T28" s="12"/>
       <c r="U28" s="10"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="13"/>
       <c r="C29" s="14"/>
@@ -2678,7 +2701,7 @@
       <c r="T29" s="12"/>
       <c r="U29" s="10"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="13"/>
       <c r="C30" s="14"/>
@@ -2701,7 +2724,7 @@
       <c r="T30" s="12"/>
       <c r="U30" s="10"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14"/>
@@ -2724,7 +2747,7 @@
       <c r="T31" s="12"/>
       <c r="U31" s="10"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
@@ -2747,7 +2770,7 @@
       <c r="T32" s="12"/>
       <c r="U32" s="10"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
@@ -2770,7 +2793,7 @@
       <c r="T33" s="12"/>
       <c r="U33" s="10"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14"/>
@@ -2793,7 +2816,7 @@
       <c r="T34" s="12"/>
       <c r="U34" s="10"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14"/>
@@ -2816,7 +2839,7 @@
       <c r="T35" s="12"/>
       <c r="U35" s="10"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
@@ -2839,7 +2862,7 @@
       <c r="T36" s="12"/>
       <c r="U36" s="10"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="13"/>
       <c r="C37" s="14"/>
@@ -2862,7 +2885,7 @@
       <c r="T37" s="12"/>
       <c r="U37" s="10"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14"/>
@@ -2885,7 +2908,7 @@
       <c r="T38" s="12"/>
       <c r="U38" s="10"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="13"/>
       <c r="C39" s="14"/>
@@ -2908,7 +2931,7 @@
       <c r="T39" s="12"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
@@ -2931,7 +2954,7 @@
       <c r="T40" s="12"/>
       <c r="U40" s="10"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
@@ -2954,7 +2977,7 @@
       <c r="T41" s="12"/>
       <c r="U41" s="10"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
@@ -2977,7 +3000,7 @@
       <c r="T42" s="12"/>
       <c r="U42" s="10"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
@@ -3000,7 +3023,7 @@
       <c r="T43" s="12"/>
       <c r="U43" s="10"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
@@ -3023,7 +3046,7 @@
       <c r="T44" s="12"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
@@ -3046,7 +3069,7 @@
       <c r="T45" s="12"/>
       <c r="U45" s="10"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
@@ -3069,7 +3092,7 @@
       <c r="T46" s="12"/>
       <c r="U46" s="10"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
@@ -3092,7 +3115,7 @@
       <c r="T47" s="12"/>
       <c r="U47" s="10"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
@@ -3115,7 +3138,7 @@
       <c r="T48" s="12"/>
       <c r="U48" s="10"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
@@ -3138,7 +3161,7 @@
       <c r="T49" s="12"/>
       <c r="U49" s="10"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
@@ -3161,7 +3184,7 @@
       <c r="T50" s="12"/>
       <c r="U50" s="10"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
@@ -3184,7 +3207,7 @@
       <c r="T51" s="12"/>
       <c r="U51" s="10"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
@@ -3207,7 +3230,7 @@
       <c r="T52" s="12"/>
       <c r="U52" s="10"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
@@ -3230,7 +3253,7 @@
       <c r="T53" s="12"/>
       <c r="U53" s="10"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
@@ -3253,7 +3276,7 @@
       <c r="T54" s="12"/>
       <c r="U54" s="10"/>
     </row>
-    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
@@ -3276,7 +3299,7 @@
       <c r="T55" s="12"/>
       <c r="U55" s="10"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
@@ -3299,7 +3322,7 @@
       <c r="T56" s="12"/>
       <c r="U56" s="10"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
@@ -3322,7 +3345,7 @@
       <c r="T57" s="12"/>
       <c r="U57" s="10"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
@@ -3345,7 +3368,7 @@
       <c r="T58" s="12"/>
       <c r="U58" s="10"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
@@ -3368,7 +3391,7 @@
       <c r="T59" s="12"/>
       <c r="U59" s="10"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
@@ -3391,7 +3414,7 @@
       <c r="T60" s="12"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
@@ -3414,7 +3437,7 @@
       <c r="T61" s="12"/>
       <c r="U61" s="10"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
@@ -3437,7 +3460,7 @@
       <c r="T62" s="12"/>
       <c r="U62" s="10"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14"/>
@@ -3460,7 +3483,7 @@
       <c r="T63" s="12"/>
       <c r="U63" s="10"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14"/>
@@ -3483,7 +3506,7 @@
       <c r="T64" s="12"/>
       <c r="U64" s="10"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14"/>
@@ -3506,7 +3529,7 @@
       <c r="T65" s="12"/>
       <c r="U65" s="10"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
@@ -3529,7 +3552,7 @@
       <c r="T66" s="12"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14"/>
@@ -3552,7 +3575,7 @@
       <c r="T67" s="12"/>
       <c r="U67" s="10"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14"/>
@@ -3575,7 +3598,7 @@
       <c r="T68" s="12"/>
       <c r="U68" s="10"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14"/>
@@ -3598,7 +3621,7 @@
       <c r="T69" s="12"/>
       <c r="U69" s="10"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14"/>
@@ -3621,7 +3644,7 @@
       <c r="T70" s="12"/>
       <c r="U70" s="10"/>
     </row>
-    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14"/>
@@ -3644,7 +3667,7 @@
       <c r="T71" s="12"/>
       <c r="U71" s="10"/>
     </row>
-    <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14"/>
@@ -3667,378 +3690,372 @@
       <c r="T72" s="12"/>
       <c r="U72" s="10"/>
     </row>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="129" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="130" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="131" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="132" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="133" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="134" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="135" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="136" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="137" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="138" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="139" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="140" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="141" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="142" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="143" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="144" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="135" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="136" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="137" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="138" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="139" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="140" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="141" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="142" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="143" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="144" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:U24">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4053,6 +4070,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O5" r:id="rId1"/>
@@ -4115,27 +4138,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="2" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="2"/>
-    <col min="14" max="14" width="24.265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="2"/>
+    <col min="13" max="13" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="24.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -4152,7 +4175,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -4176,7 +4199,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -4195,7 +4218,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -4214,7 +4237,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -4230,7 +4253,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -4247,7 +4270,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -4264,7 +4287,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4279,7 +4302,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -4294,7 +4317,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4309,7 +4332,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4324,7 +4347,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -4339,7 +4362,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -4354,7 +4377,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -4369,7 +4392,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -4384,7 +4407,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -4399,7 +4422,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
@@ -4413,7 +4436,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
@@ -4427,7 +4450,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
@@ -4441,7 +4464,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
@@ -4455,7 +4478,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -4470,7 +4493,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -4485,7 +4508,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -4500,7 +4523,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -4515,7 +4538,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -4530,7 +4553,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -4545,7 +4568,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -4560,7 +4583,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -4575,7 +4598,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -4590,7 +4613,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -4605,7 +4628,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -4620,7 +4643,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -4635,7 +4658,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -4650,7 +4673,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -4665,7 +4688,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -4680,7 +4703,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -4695,7 +4718,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -4710,7 +4733,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -4725,7 +4748,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -4740,7 +4763,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -4755,7 +4778,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -4770,7 +4793,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -4785,7 +4808,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -4800,7 +4823,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -4815,7 +4838,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -4830,7 +4853,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -4845,7 +4868,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -4860,7 +4883,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -4875,7 +4898,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -4887,7 +4910,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -4899,7 +4922,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -4912,7 +4935,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -4925,7 +4948,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -4938,7 +4961,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -4951,7 +4974,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -4964,7 +4987,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -4977,7 +5000,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -4990,7 +5013,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -5003,7 +5026,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -5016,7 +5039,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -5029,7 +5052,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -5042,7 +5065,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -5055,7 +5078,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -5068,7 +5091,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -5081,7 +5104,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -5094,7 +5117,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -5107,7 +5130,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -5120,7 +5143,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -5133,7 +5156,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -5146,7 +5169,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -5159,7 +5182,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -5173,7 +5196,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -5187,7 +5210,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -5201,7 +5224,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -5215,7 +5238,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -5229,7 +5252,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5243,7 +5266,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5257,7 +5280,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5271,7 +5294,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5285,7 +5308,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5299,7 +5322,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5313,7 +5336,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5327,7 +5350,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5341,7 +5364,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5355,7 +5378,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5369,7 +5392,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5383,7 +5406,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5397,7 +5420,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5411,7 +5434,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5425,7 +5448,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5439,7 +5462,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5453,7 +5476,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5467,7 +5490,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5481,7 +5504,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5495,7 +5518,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5509,7 +5532,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5523,7 +5546,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5537,7 +5560,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5551,7 +5574,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5565,7 +5588,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5579,7 +5602,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5593,7 +5616,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -5607,7 +5630,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5621,7 +5644,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -5635,7 +5658,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5649,7 +5672,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -5663,7 +5686,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5677,7 +5700,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -5691,7 +5714,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5705,7 +5728,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -5719,7 +5742,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -5733,7 +5756,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -5747,7 +5770,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -5761,7 +5784,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -5775,7 +5798,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -5789,7 +5812,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -5803,7 +5826,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -5817,7 +5840,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -5831,7 +5854,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -5845,7 +5868,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -5859,7 +5882,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -5873,7 +5896,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -5887,7 +5910,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -5901,7 +5924,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -5915,7 +5938,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -5929,7 +5952,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -5943,7 +5966,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -5957,7 +5980,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -5971,7 +5994,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -5985,7 +6008,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -5999,7 +6022,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -6013,7 +6036,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -6027,7 +6050,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>

</xml_diff>